<commit_message>
filtered usable parameter in explanation file and process ammo names
</commit_message>
<xml_diff>
--- a/LaTeX/data/bf1-weapons/parameter_explanation.xlsx
+++ b/LaTeX/data/bf1-weapons/parameter_explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game Development\MasterThesis\LaTeX branch\LaTeX\data\bf1-weapons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{28AB71B6-188E-4A96-85BF-183810FA8F8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{48145141-0A71-4199-81F6-954F137D52DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{0939B271-64B0-4DB5-BCC6-D713B32E088D}"/>
   </bookViews>
@@ -583,7 +583,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,8 +605,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -616,12 +630,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,13 +672,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -987,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A776FC9F-C7F6-4055-8EF3-C395D2A1A156}">
   <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,731 +1018,731 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="4" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="4" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="4" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="4" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="7" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="4" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+    <row r="73" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+    <row r="78" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+    <row r="79" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+    <row r="80" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+    <row r="81" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+    <row r="83" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+    <row r="84" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+    <row r="85" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+    <row r="86" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+    <row r="87" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+    <row r="91" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="4" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created custom parameter extraction script added some thoughts in latex changed parameter description in explanation spreadsheet
</commit_message>
<xml_diff>
--- a/LaTeX/data/bf1-weapons/parameter_explanation.xlsx
+++ b/LaTeX/data/bf1-weapons/parameter_explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game Development\MasterThesis\LaTeX branch\LaTeX\data\bf1-weapons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{48145141-0A71-4199-81F6-954F137D52DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2F291B02-5309-4737-ACD0-D266A14FD917}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{0939B271-64B0-4DB5-BCC6-D713B32E088D}"/>
   </bookViews>
@@ -360,9 +360,6 @@
     <t>Damage points applied, listed based on distance.</t>
   </si>
   <si>
-    <t>Distances for correlation damage entry.</t>
-  </si>
-  <si>
     <t>Decrease of shot spread if character is crouching, moving, and is aiming down sight.</t>
   </si>
   <si>
@@ -468,12 +465,6 @@
     <t>Weapon recoil decrease if character is NOT aiming down sight.</t>
   </si>
   <si>
-    <t>Weapon recoil to the left if character is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Weapon recoil to the right if character is NOT aiming down sight.</t>
-  </si>
-  <si>
     <t>Weapon recoil upwards if character is NOT aiming down sight.</t>
   </si>
   <si>
@@ -540,18 +531,12 @@
     <t>Least applied damage points.</t>
   </si>
   <si>
-    <t>Time it takes to reload single bullets after "FirstSingleBulletTime" was applied.</t>
-  </si>
-  <si>
     <t>Time it takes to reload the stripper clip.</t>
   </si>
   <si>
     <t>Remnant parameter gathered by scripts.</t>
   </si>
   <si>
-    <t>The weapon's class such as, e.g. pistol or rifle.</t>
-  </si>
-  <si>
     <t>Number of bullets reloaded when using magazines or strip clips.</t>
   </si>
   <si>
@@ -577,6 +562,21 @@
   </si>
   <si>
     <t>Time it takes to reload the first bullet if single bullets can be reloaded.</t>
+  </si>
+  <si>
+    <t>Defines which character class in BF1 uses this weapon</t>
+  </si>
+  <si>
+    <t>Time it takes to reload single bullets after "FirstSingleBulletTime" was applied. (Semi-automatic and bolt-action weapons)</t>
+  </si>
+  <si>
+    <t>Weapon recoil lower bound of random recoil if character is NOT aiming down sight.</t>
+  </si>
+  <si>
+    <t>Weapon recoil upper bound of random recoil if character is NOT aiming down sight.</t>
+  </si>
+  <si>
+    <t>Distances in correlation to each damage entry in Damages parameter.</t>
   </si>
 </sst>
 </file>
@@ -620,18 +620,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -672,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -682,7 +676,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A776FC9F-C7F6-4055-8EF3-C395D2A1A156}">
   <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1008,7 @@
         <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1023,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1031,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1039,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1047,7 +1040,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1071,7 +1064,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1079,42 +1072,42 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1122,7 +1115,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1130,20 +1123,20 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1183,7 +1176,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1191,7 +1184,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1199,7 +1192,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1207,7 +1200,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1231,7 +1224,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1239,7 +1232,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1247,7 +1240,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1255,7 +1248,7 @@
         <v>91</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1263,7 +1256,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1279,15 +1272,15 @@
         <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>174</v>
+      <c r="B35" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1303,7 +1296,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1311,7 +1304,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1319,7 +1312,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1327,7 +1320,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1335,7 +1328,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1343,7 +1336,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1351,7 +1344,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1359,7 +1352,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1367,7 +1360,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1375,7 +1368,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1383,7 +1376,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1391,7 +1384,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1399,7 +1392,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1407,7 +1400,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1415,7 +1408,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1423,7 +1416,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1431,7 +1424,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,7 +1432,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1447,7 +1440,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1455,7 +1448,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1463,7 +1456,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1471,7 +1464,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1479,7 +1472,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1487,7 +1480,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1495,7 +1488,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1503,7 +1496,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1511,7 +1504,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1519,7 +1512,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1527,7 +1520,7 @@
         <v>62</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1535,7 +1528,7 @@
         <v>63</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1543,7 +1536,7 @@
         <v>64</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1551,7 +1544,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1559,7 +1552,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1567,7 +1560,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1575,7 +1568,7 @@
         <v>68</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1583,7 +1576,7 @@
         <v>69</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1599,7 +1592,7 @@
         <v>71</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1615,7 +1608,7 @@
         <v>73</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="77" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1623,7 +1616,7 @@
         <v>74</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1631,7 +1624,7 @@
         <v>75</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1639,7 +1632,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1647,7 +1640,7 @@
         <v>77</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1655,7 +1648,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1671,7 +1664,7 @@
         <v>80</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1690,12 +1683,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
+    <row r="86" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B86" s="4" t="s">
-        <v>171</v>
+      <c r="B86" s="7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1703,7 +1696,7 @@
         <v>84</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1711,7 +1704,7 @@
         <v>85</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1719,7 +1712,7 @@
         <v>86</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1730,7 +1723,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>88</v>
       </c>
@@ -1738,12 +1731,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="92" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed hipstandmovemax, hipstandmovespreaddec and hipstandmovespreadinc from used parameters
</commit_message>
<xml_diff>
--- a/LaTeX/data/bf1-weapons/parameter_explanation.xlsx
+++ b/LaTeX/data/bf1-weapons/parameter_explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game Development\MasterThesis\LaTeX branch\LaTeX\data\bf1-weapons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2F291B02-5309-4737-ACD0-D266A14FD917}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{702BF8D6-B2A0-4964-86CE-49540FEAE20A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{0939B271-64B0-4DB5-BCC6-D713B32E088D}"/>
   </bookViews>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A776FC9F-C7F6-4055-8EF3-C395D2A1A156}">
   <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,10 +1252,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="4" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1548,10 +1548,10 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1564,18 +1564,18 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="4" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="4" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed some folder names; updated weapon dump parameter explanations; added the explanations in latex; wrote the beginning in the prototype development chapter
</commit_message>
<xml_diff>
--- a/LaTeX/data/bf1-weapons/parameter_explanation.xlsx
+++ b/LaTeX/data/bf1-weapons/parameter_explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game Development\MasterThesis\LaTeX branch\LaTeX\data\bf1-weapons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D785DA75-8B5F-4F20-953D-96302825C67D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E06D8211-4E80-4FF2-8AA3-D86DBFB1C925}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{0939B271-64B0-4DB5-BCC6-D713B32E088D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="185">
   <si>
     <t>ADSProneBaseMin</t>
   </si>
@@ -303,54 +303,12 @@
     <t>Ammo</t>
   </si>
   <si>
-    <t>Weapon recoil decrease if character is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character is crouching, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character is crouching, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character prones, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character prones, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Weapon recoil to the left if character is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Weapon recoil to the right if character is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Weapon recoil upwards if character is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character is standing, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character is standing, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Rate of fire in burst mode.</t>
-  </si>
-  <si>
     <t>Horizontal pellet dispersion (for shotguns).</t>
   </si>
   <si>
     <t>Vertical pellet dispersion (for shotguns).</t>
   </si>
   <si>
-    <t>Number of pellets of one shot in burst mode.</t>
-  </si>
-  <si>
-    <t>Number of pellets of one shot.</t>
-  </si>
-  <si>
-    <t>Rate of fire.</t>
-  </si>
-  <si>
     <t>Size of one magazine.</t>
   </si>
   <si>
@@ -360,186 +318,27 @@
     <t>Damage points applied, listed based on distance.</t>
   </si>
   <si>
-    <t>Decrease of shot spread if character is crouching, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character prones, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character is standing, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character is crouching, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character prones, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character is standing, moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character is crouching, NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character is crouching, NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character is crouching, NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character is crouching, NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character prones, is NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character prones, is NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character prones, is NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character prones, is NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character is standing, NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character is standing, NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character is standing, NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character is standing, NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character is crouching, NOT moving, and is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character is crouching, NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character is crouching, NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character is crouching, NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character is crouching, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character is crouching, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character is crouching, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character is crouching, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character prones, is NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character prones, is NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character prones, is NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character prones, is NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character prones, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character prones, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character prones, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character prones, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Weapon recoil decrease if character is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Weapon recoil upwards if character is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character is standing, NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character is standing, NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character is standing, NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character is standing, NOT moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Maximum shot spread if character is standing, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Minimum shot spread if character is standing, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Decrease of shot spread if character is standing, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Increase of shot spread if character is standing, moving, and is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Type of ammunition used.</t>
-  </si>
-  <si>
     <t>A bullet's drag.</t>
   </si>
   <si>
     <t>Is the time it takes to weapon be able to fire after switching to said weapon.</t>
   </si>
   <si>
-    <t>Delay added to first single bullet being reloaded.</t>
-  </si>
-  <si>
     <t>Muzzle velocity.</t>
   </si>
   <si>
     <t>A bullet's drop due to gravity.</t>
   </si>
   <si>
-    <t>Tells the fraction of how much of the reload has to be done before you can swap weapons and still have completed reload.</t>
-  </si>
-  <si>
-    <t>Time it takes if the magazine is empty.</t>
-  </si>
-  <si>
-    <t>Time it takes if the magazine there is still some ammo left.</t>
-  </si>
-  <si>
     <t>Is applied when different reload-times/ reload types can happen depending on how many bullets are in the weapon.</t>
   </si>
   <si>
-    <t>Post-reload delay after reloading mechnic ends.</t>
-  </si>
-  <si>
     <t>Explanation</t>
   </si>
   <si>
     <t>Least applied damage points.</t>
   </si>
   <si>
-    <t>Time it takes to reload the stripper clip.</t>
-  </si>
-  <si>
-    <t>Remnant parameter gathered by scripts.</t>
-  </si>
-  <si>
-    <t>Number of bullets reloaded when using magazines or strip clips.</t>
-  </si>
-  <si>
     <t>Pre-reload delay before actual reloading mechanic begins. (Not strip clip reload or single bullet reload)</t>
   </si>
   <si>
@@ -549,34 +348,238 @@
     <t>Seconds how long the bullet lives before despawning.</t>
   </si>
   <si>
-    <t>Spread multiplier applied on first shot or the final shot in burst mode if character is aiming down sight.</t>
-  </si>
-  <si>
-    <t>Recoil multiplier applied on first shot or the final shot in burst mode.</t>
-  </si>
-  <si>
-    <t>Spread multiplier applied on first shot or the final shot in burst mode if character is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Number of bullets reloaded by "strip" clips.</t>
-  </si>
-  <si>
-    <t>Time it takes to reload the first bullet if single bullets can be reloaded.</t>
-  </si>
-  <si>
-    <t>Defines which character class in BF1 uses this weapon</t>
-  </si>
-  <si>
-    <t>Time it takes to reload single bullets after "FirstSingleBulletTime" was applied. (Semi-automatic and bolt-action weapons)</t>
-  </si>
-  <si>
-    <t>Weapon recoil lower bound of random recoil if character is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Weapon recoil upper bound of random recoil if character is NOT aiming down sight.</t>
-  </si>
-  <si>
-    <t>Distances in correlation to each damage entry in Damages parameter.</t>
+    <t>Weapon recoil decrease if the character is aiming down sight.</t>
+  </si>
+  <si>
+    <t>Weapon recoil to the left if the character is aiming down sight.</t>
+  </si>
+  <si>
+    <t>Weapon recoil to the right if the character is aiming down sight.</t>
+  </si>
+  <si>
+    <t>Weapon recoil upwards if the character is aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is crouching, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is crouching, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is crouching, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is crouching, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is lying, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is lying, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is lying, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is lying, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is standing, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is standing, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is standing, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is standing, moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Defines which character class in Battlefield 1 uses this weapon.</t>
+  </si>
+  <si>
+    <t>Type of ammunition used in the weapon.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is crouching, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is crouching, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is crouching, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is crouching, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is lying, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is lying, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is lying, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is lying, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is standing, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is standing, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is standing, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is standing, not moving, and aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is crouching, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is crouching, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is crouching, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is crouching, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is crouching, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is crouching, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is crouching, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is lying, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is lying, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is lying, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is lying, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is lying, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is lying, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Weapon recoil decrease if the character is not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Weapon recoil upwards if the character is not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is standing, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is standing, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is standing, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is standing, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Maximum shot spread if the character is standing, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Minimum shot spread if the character is standing, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The decrease of shot spread if the character is standing, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is standing, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Remnant parameter gathered by the script.</t>
+  </si>
+  <si>
+    <t>The rate of fire in burst mode.</t>
+  </si>
+  <si>
+    <t>Delay added to the first reloaded single bullet.</t>
+  </si>
+  <si>
+    <t>The distances in correlation to each damage entry in the "Damages" parameter.</t>
+  </si>
+  <si>
+    <t>Spread multiplier applied on the first shot or the final shot in burst mode if the character is aiming down sight.</t>
+  </si>
+  <si>
+    <t>Spread multiplier applied on the first shot or the final shot in burst mode if the character is not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Recoil multiplier applied on the first shot or the final shot in burst mode.</t>
+  </si>
+  <si>
+    <t>The time it takes to reload the first bullet if single bullet reloading is available.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is crouching, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is lying, not moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The increase of shot spread if the character is lying, moving, and not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Weapon recoil lower bound of random recoil if the character is not aiming down sight.</t>
+  </si>
+  <si>
+    <t>Weapon recoil upper bound of random recoil if the character is not aiming down sight.</t>
+  </si>
+  <si>
+    <t>The Number of bullets reloaded when using magazines or strip clips.</t>
+  </si>
+  <si>
+    <t>Post-reload delay after reloading mechanic ends.</t>
+  </si>
+  <si>
+    <t>The time it takes if the magazine is empty.</t>
+  </si>
+  <si>
+    <t>The time it takes if the magazine there is still some ammo left.</t>
+  </si>
+  <si>
+    <t>The fraction of the reload time before someone can swap weapons and still receives fully reloaded ammo.</t>
+  </si>
+  <si>
+    <t>The rate of fire.</t>
+  </si>
+  <si>
+    <t>The number of pellets of one shot in burst mode.</t>
+  </si>
+  <si>
+    <t>The number of pellets of one shot.</t>
+  </si>
+  <si>
+    <t>The time it takes to reload single bullets after "FirstSingleBulletTime" was applied. (Semi-automatic and bolt-action weapons)</t>
+  </si>
+  <si>
+    <t>The time it takes to reload the stripper clip.</t>
+  </si>
+  <si>
+    <t>The number of bullets reloaded by "strip" clips.</t>
+  </si>
+  <si>
+    <t>This parameter only applies in super individual cases.</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -651,17 +654,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -674,7 +666,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -989,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A776FC9F-C7F6-4055-8EF3-C395D2A1A156}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +998,7 @@
         <v>90</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>166</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1014,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1022,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1030,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1038,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1046,7 +1038,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1054,7 +1046,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1062,7 +1054,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1078,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1086,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1094,7 +1086,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1102,7 +1094,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1110,7 +1102,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1118,7 +1110,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1126,7 +1118,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1134,7 +1126,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1142,7 +1134,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1150,7 +1142,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,7 +1150,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1166,7 +1158,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1174,7 +1166,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1182,7 +1174,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1190,7 +1182,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1198,7 +1190,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,7 +1198,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1214,7 +1206,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1222,7 +1214,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1230,7 +1222,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1238,7 +1230,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1246,7 +1238,7 @@
         <v>91</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1254,7 +1246,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>160</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1262,7 +1254,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1270,7 +1262,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1278,7 +1270,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>179</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1286,7 +1278,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1294,7 +1286,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1302,7 +1294,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1310,7 +1302,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1318,7 +1310,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1326,7 +1318,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1334,7 +1326,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1342,7 +1334,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1350,7 +1342,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1358,7 +1350,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1366,7 +1358,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1374,7 +1366,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1382,7 +1374,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1390,7 +1382,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1398,7 +1390,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1406,7 +1398,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1414,7 +1406,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1422,7 +1414,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,7 +1422,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1438,7 +1430,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1446,7 +1438,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1454,7 +1446,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1462,7 +1454,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1470,7 +1462,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1478,7 +1470,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1486,7 +1478,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1494,7 +1486,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1502,7 +1494,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1510,7 +1502,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1518,7 +1510,7 @@
         <v>62</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1526,7 +1518,7 @@
         <v>63</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1534,7 +1526,7 @@
         <v>64</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1542,7 +1534,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1550,7 +1542,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1558,7 +1550,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1566,7 +1558,7 @@
         <v>68</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1574,7 +1566,7 @@
         <v>69</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1582,7 +1574,7 @@
         <v>70</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1590,7 +1582,7 @@
         <v>71</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>159</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1598,7 +1590,7 @@
         <v>72</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1606,15 +1598,15 @@
         <v>73</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>165</v>
+      <c r="B77" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1622,7 +1614,7 @@
         <v>75</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>171</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1630,7 +1622,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1638,7 +1630,7 @@
         <v>77</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1646,7 +1638,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1654,7 +1646,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1662,7 +1654,7 @@
         <v>80</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1670,7 +1662,7 @@
         <v>81</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>105</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1678,7 +1670,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>106</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1686,7 +1678,7 @@
         <v>83</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="87" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1694,7 +1686,7 @@
         <v>84</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1702,7 +1694,7 @@
         <v>85</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="89" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1710,7 +1702,7 @@
         <v>86</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>173</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1718,7 +1710,7 @@
         <v>87</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:2" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1726,7 +1718,7 @@
         <v>88</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:2" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -1734,7 +1726,15 @@
         <v>89</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>164</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>